<commit_message>
add_phase action bug fix
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912A6F8C-567D-4227-9095-315B48FE754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B63CD0-BE2E-4717-B9E1-C8A735F279F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -939,18 +939,12 @@
     <t>[{"phase_name":"Amendment Application Review (Typical)","work_type_id":7,"ea_act_id":3,"is_active":false}]</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Simple) (Date Capture)", "start_at": 1 }</t>
   </si>
   <si>
     <t>{"phase_name":"Amendment Application Review (Typical)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Typical) (Date Capture)", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Complex)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Complex) (Date Capture)", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Amendment</t>
   </si>
   <si>
@@ -963,10 +957,16 @@
     <t>AddPhase</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Complex)","work_type_id":7,"ea_act_id":3, "new_name": "Amendment Application Review (Complex)", "legislated": false}</t>
-  </si>
-  <si>
     <t>{"work_type":15}</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Review (Complex)","work_type_id":7,"ea_act_id":3, "new_name": "Revised Amendment Application Review (Complex)", "legislated": false}]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised Amendment Application Review (Complex)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Complex) (Date Capture)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }]</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1668,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1697,7 +1697,7 @@
         <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1726,7 +1726,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1755,7 +1755,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1784,7 +1784,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1813,7 +1813,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1842,7 +1842,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
@@ -1871,7 +1871,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -9727,7 +9727,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9855,7 +9855,7 @@
         <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -10023,7 +10023,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -10047,7 +10047,7 @@
         <v>208</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -10119,7 +10119,7 @@
         <v>203</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
@@ -10383,7 +10383,7 @@
         <v>203</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
@@ -10569,13 +10569,13 @@
         <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>218</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
@@ -10599,7 +10599,7 @@
         <v>221</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="3">
         <v>35</v>
@@ -10623,7 +10623,7 @@
         <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
@@ -10665,13 +10665,13 @@
         <v>Amendment is determined to be "Complex"</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>219</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G39" s="3">
         <v>38</v>
@@ -10695,7 +10695,7 @@
         <v>222</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="G40" s="3">
         <v>39</v>
@@ -10719,7 +10719,7 @@
         <v>203</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G41" s="3">
         <v>40</v>
@@ -10887,7 +10887,7 @@
         <v>203</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G48" s="3">
         <v>47</v>
@@ -11055,7 +11055,7 @@
         <v>203</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G55" s="3">
         <v>54</v>

</xml_diff>

<commit_message>
add_phase action bug fix (#1344)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912A6F8C-567D-4227-9095-315B48FE754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B63CD0-BE2E-4717-B9E1-C8A735F279F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -939,18 +939,12 @@
     <t>[{"phase_name":"Amendment Application Review (Typical)","work_type_id":7,"ea_act_id":3,"is_active":false}]</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Simple) (Date Capture)", "start_at": 1 }</t>
   </si>
   <si>
     <t>{"phase_name":"Amendment Application Review (Typical)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Typical) (Date Capture)", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Complex)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Complex) (Date Capture)", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Amendment</t>
   </si>
   <si>
@@ -963,10 +957,16 @@
     <t>AddPhase</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Review (Complex)","work_type_id":7,"ea_act_id":3, "new_name": "Amendment Application Review (Complex)", "legislated": false}</t>
-  </si>
-  <si>
     <t>{"work_type":15}</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Review (Complex)","work_type_id":7,"ea_act_id":3, "new_name": "Revised Amendment Application Review (Complex)", "legislated": false}]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised Amendment Application Review (Complex)","work_type_id": 7, "ea_act_id": 3, "event_name": "Start of Amendment Application Review (Complex) (Date Capture)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }]</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1668,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1697,7 +1697,7 @@
         <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1726,7 +1726,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1755,7 +1755,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1784,7 +1784,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1813,7 +1813,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1842,7 +1842,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
@@ -1871,7 +1871,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -9727,7 +9727,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9855,7 +9855,7 @@
         <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -10023,7 +10023,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -10047,7 +10047,7 @@
         <v>208</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -10119,7 +10119,7 @@
         <v>203</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
@@ -10383,7 +10383,7 @@
         <v>203</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
@@ -10569,13 +10569,13 @@
         <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>218</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
@@ -10599,7 +10599,7 @@
         <v>221</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="3">
         <v>35</v>
@@ -10623,7 +10623,7 @@
         <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
@@ -10665,13 +10665,13 @@
         <v>Amendment is determined to be "Complex"</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>219</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G39" s="3">
         <v>38</v>
@@ -10695,7 +10695,7 @@
         <v>222</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="G40" s="3">
         <v>39</v>
@@ -10719,7 +10719,7 @@
         <v>203</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G41" s="3">
         <v>40</v>
@@ -10887,7 +10887,7 @@
         <v>203</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G48" s="3">
         <v>47</v>
@@ -11055,7 +11055,7 @@
         <v>203</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G55" s="3">
         <v>54</v>

</xml_diff>

<commit_message>
addEvent action logic + event list sorting
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B63CD0-BE2E-4717-B9E1-C8A735F279F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD980EA4-B3C4-42B1-8728-5EDE39A9633A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="249">
   <si>
     <t>No</t>
   </si>
@@ -843,12 +843,6 @@
     <t>Set ANTICIPATED of "Amendment Application Submission | Amendment Application Received" to thisEventACTUAL +1</t>
   </si>
   <si>
-    <t>Add a copy of "Amendment Application Development (Proponent Time) | Submission of "Draft" Amendment Application" to thisPhase at thisEventACTUAL +28</t>
-  </si>
-  <si>
-    <t>Add a copy of "Amendment Application Development (Proponent Time) | "Draft" Amendment Application Initial Review" to thisPhase at thisEventACTUAL +38</t>
-  </si>
-  <si>
     <t>LockWorkStartDate</t>
   </si>
   <si>
@@ -906,12 +900,6 @@
     <t>{"work_state": "TERMINATED"}</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Amendment Application", "start_at": 28 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "\"Draft\" Amendment Application Initial Review", "start_at": 38 }</t>
-  </si>
-  <si>
     <t>{"start_date_locked": true}</t>
   </si>
   <si>
@@ -967,6 +955,12 @@
   </si>
   <si>
     <t>[{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Amendment Application", "start_at": 28 },{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "\"Draft\" Amendment Application Initial Review", "start_at": 10}]</t>
+  </si>
+  <si>
+    <t>Add a copy of "Amendment Application Development (Proponent Time) | Submission of "Draft" Amendment Application, "Draft" Amendment Application Initial Review" to thisPhase at thisEventACTUAL +28</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1648,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1668,7 +1662,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1683,7 +1677,7 @@
         <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1697,7 +1691,7 @@
         <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1712,7 +1706,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1726,7 +1720,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1741,7 +1735,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I4" s="3">
         <v>3</v>
@@ -1755,7 +1749,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1770,7 +1764,7 @@
         <v>65</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -1784,7 +1778,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1799,7 +1793,7 @@
         <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
@@ -1813,7 +1807,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1828,7 +1822,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
@@ -1842,7 +1836,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
@@ -1857,7 +1851,7 @@
         <v>65</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I8" s="3">
         <v>7</v>
@@ -1871,7 +1865,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -1886,7 +1880,7 @@
         <v>65</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I9" s="3">
         <v>8</v>
@@ -2584,7 +2578,7 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
@@ -2623,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M2" s="3">
         <v>1</v>
@@ -2662,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -2701,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
@@ -2740,7 +2734,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M5" s="3">
         <v>4</v>
@@ -2779,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M6" s="3">
         <v>5</v>
@@ -2818,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M7" s="3">
         <v>6</v>
@@ -2857,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M8" s="3">
         <v>7</v>
@@ -2896,7 +2890,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M9" s="3">
         <v>8</v>
@@ -2935,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M10" s="3">
         <v>9</v>
@@ -2974,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M11" s="3">
         <v>10</v>
@@ -3013,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M12" s="3">
         <v>11</v>
@@ -3052,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M13" s="3">
         <v>12</v>
@@ -3091,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M14" s="3">
         <v>13</v>
@@ -3130,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M15" s="3">
         <v>14</v>
@@ -3172,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M16" s="3">
         <v>15</v>
@@ -3214,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M17" s="3">
         <v>16</v>
@@ -3253,7 +3247,7 @@
         <v>30</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M18" s="3">
         <v>17</v>
@@ -3295,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M19" s="3">
         <v>18</v>
@@ -3337,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M20" s="3">
         <v>19</v>
@@ -3379,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M21" s="3">
         <v>20</v>
@@ -3421,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M22" s="3">
         <v>21</v>
@@ -3460,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M23" s="3">
         <v>22</v>
@@ -3499,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M24" s="3">
         <v>23</v>
@@ -3538,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M25" s="3">
         <v>24</v>
@@ -3580,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M26" s="3">
         <v>25</v>
@@ -3622,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M27" s="3">
         <v>26</v>
@@ -3661,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M28" s="3">
         <v>27</v>
@@ -3703,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M29" s="3">
         <v>28</v>
@@ -3745,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M30" s="3">
         <v>29</v>
@@ -3784,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M31" s="3">
         <v>30</v>
@@ -3826,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M32" s="3">
         <v>31</v>
@@ -3868,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M33" s="3">
         <v>32</v>
@@ -3907,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M34" s="3">
         <v>33</v>
@@ -3946,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M35" s="3">
         <v>34</v>
@@ -3988,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M36" s="3">
         <v>35</v>
@@ -4030,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M37" s="3">
         <v>36</v>
@@ -4069,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M38" s="3">
         <v>37</v>
@@ -4108,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M39" s="3">
         <v>38</v>
@@ -4147,7 +4141,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M40" s="3">
         <v>39</v>
@@ -4186,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M41" s="3">
         <v>40</v>
@@ -4225,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M42" s="3">
         <v>41</v>
@@ -4264,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M43" s="3">
         <v>42</v>
@@ -4303,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M44" s="3">
         <v>43</v>
@@ -4345,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M45" s="3">
         <v>44</v>
@@ -4387,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M46" s="3">
         <v>45</v>
@@ -4426,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M47" s="3">
         <v>46</v>
@@ -4468,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M48" s="3">
         <v>47</v>
@@ -4510,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M49" s="3">
         <v>48</v>
@@ -4549,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M50" s="3">
         <v>49</v>
@@ -4591,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M51" s="3">
         <v>50</v>
@@ -4633,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M52" s="3">
         <v>51</v>
@@ -4672,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M53" s="3">
         <v>52</v>
@@ -4711,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M54" s="3">
         <v>53</v>
@@ -4750,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M55" s="3">
         <v>54</v>
@@ -4792,7 +4786,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M56" s="3">
         <v>55</v>
@@ -4834,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M57" s="3">
         <v>56</v>
@@ -4873,7 +4867,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M58" s="3">
         <v>57</v>
@@ -4912,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M59" s="3">
         <v>58</v>
@@ -4954,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M60" s="3">
         <v>59</v>
@@ -4993,7 +4987,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M61" s="3">
         <v>60</v>
@@ -5032,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M62" s="3">
         <v>61</v>
@@ -5071,7 +5065,7 @@
         <v>0</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M63" s="3">
         <v>62</v>
@@ -5113,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M64" s="3">
         <v>63</v>
@@ -5155,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M65" s="3">
         <v>64</v>
@@ -5194,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M66" s="3">
         <v>65</v>
@@ -5236,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M67" s="3">
         <v>66</v>
@@ -5278,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M68" s="3">
         <v>67</v>
@@ -5317,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M69" s="3">
         <v>68</v>
@@ -5359,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M70" s="3">
         <v>69</v>
@@ -5401,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M71" s="3">
         <v>70</v>
@@ -5440,7 +5434,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M72" s="3">
         <v>71</v>
@@ -5479,7 +5473,7 @@
         <v>0</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M73" s="3">
         <v>72</v>
@@ -5518,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M74" s="3">
         <v>73</v>
@@ -5557,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M75" s="3">
         <v>74</v>
@@ -5596,7 +5590,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M76" s="3">
         <v>75</v>
@@ -5635,7 +5629,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M77" s="3">
         <v>76</v>
@@ -5674,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M78" s="3">
         <v>77</v>
@@ -5716,7 +5710,7 @@
         <v>0</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M79" s="3">
         <v>78</v>
@@ -5758,7 +5752,7 @@
         <v>0</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M80" s="3">
         <v>79</v>
@@ -5797,7 +5791,7 @@
         <v>30</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M81" s="3">
         <v>80</v>
@@ -5839,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M82" s="3">
         <v>81</v>
@@ -5881,7 +5875,7 @@
         <v>0</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M83" s="3">
         <v>82</v>
@@ -5923,7 +5917,7 @@
         <v>0</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M84" s="3">
         <v>83</v>
@@ -5965,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M85" s="3">
         <v>84</v>
@@ -6004,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M86" s="3">
         <v>85</v>
@@ -6043,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M87" s="3">
         <v>86</v>
@@ -6082,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M88" s="3">
         <v>87</v>
@@ -6124,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M89" s="3">
         <v>88</v>
@@ -6166,7 +6160,7 @@
         <v>0</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M90" s="3">
         <v>89</v>
@@ -6205,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M91" s="3">
         <v>90</v>
@@ -6247,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M92" s="3">
         <v>91</v>
@@ -6289,7 +6283,7 @@
         <v>0</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M93" s="3">
         <v>92</v>
@@ -6328,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M94" s="3">
         <v>93</v>
@@ -6370,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M95" s="3">
         <v>94</v>
@@ -6412,7 +6406,7 @@
         <v>0</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M96" s="3">
         <v>95</v>
@@ -6451,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M97" s="3">
         <v>96</v>
@@ -6490,7 +6484,7 @@
         <v>0</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M98" s="3">
         <v>97</v>
@@ -6529,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M99" s="3">
         <v>98</v>
@@ -6568,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M100" s="3">
         <v>99</v>
@@ -6607,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M101" s="3">
         <v>100</v>
@@ -6646,7 +6640,7 @@
         <v>0</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M102" s="3">
         <v>101</v>
@@ -6685,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M103" s="3">
         <v>102</v>
@@ -6724,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="L104" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M104" s="3">
         <v>103</v>
@@ -6766,7 +6760,7 @@
         <v>0</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M105" s="3">
         <v>104</v>
@@ -6808,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M106" s="3">
         <v>105</v>
@@ -6847,7 +6841,7 @@
         <v>30</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M107" s="3">
         <v>106</v>
@@ -6889,7 +6883,7 @@
         <v>0</v>
       </c>
       <c r="L108" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M108" s="3">
         <v>107</v>
@@ -6931,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="L109" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M109" s="3">
         <v>108</v>
@@ -6973,7 +6967,7 @@
         <v>0</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M110" s="3">
         <v>109</v>
@@ -7015,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="L111" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M111" s="3">
         <v>110</v>
@@ -7054,7 +7048,7 @@
         <v>0</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M112" s="3">
         <v>111</v>
@@ -7093,7 +7087,7 @@
         <v>0</v>
       </c>
       <c r="L113" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M113" s="3">
         <v>112</v>
@@ -7132,7 +7126,7 @@
         <v>0</v>
       </c>
       <c r="L114" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M114" s="3">
         <v>113</v>
@@ -7174,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M115" s="3">
         <v>114</v>
@@ -7216,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M116" s="3">
         <v>115</v>
@@ -7255,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M117" s="3">
         <v>116</v>
@@ -7297,7 +7291,7 @@
         <v>0</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M118" s="3">
         <v>117</v>
@@ -7339,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M119" s="3">
         <v>118</v>
@@ -7378,7 +7372,7 @@
         <v>0</v>
       </c>
       <c r="L120" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M120" s="3">
         <v>119</v>
@@ -7420,7 +7414,7 @@
         <v>0</v>
       </c>
       <c r="L121" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M121" s="3">
         <v>120</v>
@@ -7462,7 +7456,7 @@
         <v>0</v>
       </c>
       <c r="L122" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M122" s="3">
         <v>121</v>
@@ -7501,7 +7495,7 @@
         <v>0</v>
       </c>
       <c r="L123" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M123" s="3">
         <v>122</v>
@@ -7540,7 +7534,7 @@
         <v>0</v>
       </c>
       <c r="L124" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M124" s="3">
         <v>123</v>
@@ -7579,7 +7573,7 @@
         <v>0</v>
       </c>
       <c r="L125" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M125" s="3">
         <v>124</v>
@@ -7618,7 +7612,7 @@
         <v>0</v>
       </c>
       <c r="L126" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M126" s="3">
         <v>125</v>
@@ -7657,7 +7651,7 @@
         <v>0</v>
       </c>
       <c r="L127" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M127" s="3">
         <v>126</v>
@@ -7696,7 +7690,7 @@
         <v>0</v>
       </c>
       <c r="L128" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M128" s="3">
         <v>127</v>
@@ -7735,7 +7729,7 @@
         <v>0</v>
       </c>
       <c r="L129" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M129" s="3">
         <v>128</v>
@@ -7774,7 +7768,7 @@
         <v>0</v>
       </c>
       <c r="L130" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M130" s="3">
         <v>129</v>
@@ -7816,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="L131" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M131" s="3">
         <v>130</v>
@@ -7858,7 +7852,7 @@
         <v>0</v>
       </c>
       <c r="L132" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M132" s="3">
         <v>131</v>
@@ -7897,7 +7891,7 @@
         <v>30</v>
       </c>
       <c r="L133" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M133" s="3">
         <v>132</v>
@@ -7939,7 +7933,7 @@
         <v>0</v>
       </c>
       <c r="L134" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M134" s="3">
         <v>133</v>
@@ -7981,7 +7975,7 @@
         <v>0</v>
       </c>
       <c r="L135" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M135" s="3">
         <v>134</v>
@@ -8023,7 +8017,7 @@
         <v>0</v>
       </c>
       <c r="L136" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M136" s="3">
         <v>135</v>
@@ -8065,7 +8059,7 @@
         <v>0</v>
       </c>
       <c r="L137" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M137" s="3">
         <v>136</v>
@@ -8104,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="L138" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M138" s="3">
         <v>137</v>
@@ -8143,7 +8137,7 @@
         <v>0</v>
       </c>
       <c r="L139" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M139" s="3">
         <v>138</v>
@@ -8182,7 +8176,7 @@
         <v>0</v>
       </c>
       <c r="L140" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M140" s="3">
         <v>139</v>
@@ -8224,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="L141" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M141" s="3">
         <v>140</v>
@@ -8266,7 +8260,7 @@
         <v>0</v>
       </c>
       <c r="L142" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M142" s="3">
         <v>141</v>
@@ -8305,7 +8299,7 @@
         <v>0</v>
       </c>
       <c r="L143" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M143" s="3">
         <v>142</v>
@@ -8347,7 +8341,7 @@
         <v>0</v>
       </c>
       <c r="L144" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M144" s="3">
         <v>143</v>
@@ -8389,7 +8383,7 @@
         <v>0</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M145" s="3">
         <v>144</v>
@@ -8428,7 +8422,7 @@
         <v>0</v>
       </c>
       <c r="L146" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M146" s="3">
         <v>145</v>
@@ -8470,7 +8464,7 @@
         <v>0</v>
       </c>
       <c r="L147" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M147" s="3">
         <v>146</v>
@@ -8512,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="L148" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M148" s="3">
         <v>147</v>
@@ -8551,7 +8545,7 @@
         <v>0</v>
       </c>
       <c r="L149" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M149" s="3">
         <v>148</v>
@@ -8590,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M150" s="3">
         <v>149</v>
@@ -8629,7 +8623,7 @@
         <v>0</v>
       </c>
       <c r="L151" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M151" s="3">
         <v>150</v>
@@ -8668,7 +8662,7 @@
         <v>0</v>
       </c>
       <c r="L152" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M152" s="3">
         <v>151</v>
@@ -8710,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="L153" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M153" s="3">
         <v>152</v>
@@ -8749,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="L154" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M154" s="3">
         <v>153</v>
@@ -8788,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="L155" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M155" s="3">
         <v>154</v>
@@ -8830,7 +8824,7 @@
         <v>0</v>
       </c>
       <c r="L156" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M156" s="3">
         <v>155</v>
@@ -8872,7 +8866,7 @@
         <v>0</v>
       </c>
       <c r="L157" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M157" s="3">
         <v>156</v>
@@ -8911,7 +8905,7 @@
         <v>0</v>
       </c>
       <c r="L158" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M158" s="3">
         <v>157</v>
@@ -8950,7 +8944,7 @@
         <v>0</v>
       </c>
       <c r="L159" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M159" s="3">
         <v>158</v>
@@ -8992,7 +8986,7 @@
         <v>0</v>
       </c>
       <c r="L160" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M160" s="3">
         <v>159</v>
@@ -9034,7 +9028,7 @@
         <v>0</v>
       </c>
       <c r="L161" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M161" s="3">
         <v>160</v>
@@ -9721,13 +9715,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9783,7 +9777,7 @@
         <v>197</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -9807,7 +9801,7 @@
         <v>199</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -9831,7 +9825,7 @@
         <v>201</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -9855,7 +9849,7 @@
         <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -9879,7 +9873,7 @@
         <v>197</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -9903,7 +9897,7 @@
         <v>199</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -9927,7 +9921,7 @@
         <v>204</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
@@ -9951,7 +9945,7 @@
         <v>197</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -9975,7 +9969,7 @@
         <v>199</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -9999,7 +9993,7 @@
         <v>201</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -10023,7 +10017,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -10047,7 +10041,7 @@
         <v>208</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -10068,10 +10062,10 @@
         <v>207</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
@@ -10079,55 +10073,55 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="str">
         <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Initial Review of "Draft" Amendment Application is NEGATIVE</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>210</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6" t="str">
         <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="8">
         <v>9</v>
@@ -10136,22 +10130,22 @@
         <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>196</v>
+      <c r="D17" t="s">
+        <v>198</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G17" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8">
         <v>9</v>
@@ -10160,46 +10154,46 @@
         <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D18" t="s">
-        <v>198</v>
+      <c r="D18" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="6" t="str">
         <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="8">
         <v>10</v>
@@ -10208,22 +10202,22 @@
         <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D20" s="26" t="s">
-        <v>196</v>
+      <c r="D20" t="s">
+        <v>198</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="8">
         <v>10</v>
@@ -10232,166 +10226,166 @@
         <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D21" t="s">
-        <v>198</v>
+      <c r="D21" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="6" t="str">
         <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Starts the "clock" for Amendment</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>210</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>228</v>
       </c>
       <c r="G22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="6" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Starts the "clock" for Amendment</v>
+        <v>ADM, EA Operations is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>211</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="6" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>ADM, EA Operations is delegated to make the final Amendment Decision</v>
+        <v>CEAO is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D24" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>216</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="6" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>CEAO is delegated to make the final Amendment Decision</v>
+        <v>Minister is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="6" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Minister is delegated to make the final Amendment Decision</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="G26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="6" t="str">
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="8">
         <v>16</v>
@@ -10400,22 +10394,22 @@
         <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>196</v>
+      <c r="D28" t="s">
+        <v>198</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="8">
         <v>16</v>
@@ -10424,46 +10418,46 @@
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D29" t="s">
-        <v>198</v>
+      <c r="D29" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="8">
         <v>17</v>
@@ -10472,22 +10466,22 @@
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D31" s="26" t="s">
-        <v>196</v>
+      <c r="D31" t="s">
+        <v>198</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="8">
         <v>17</v>
@@ -10496,46 +10490,46 @@
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D32" t="s">
-        <v>198</v>
+      <c r="D32" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="6" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="G33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="8">
         <v>18</v>
@@ -10545,21 +10539,21 @@
         <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="8">
         <v>18</v>
@@ -10568,70 +10562,70 @@
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is determined to be "Simple"</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>246</v>
+      <c r="D35" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" s="6" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Simple"</v>
+        <v>Amendment is determined to be "Typical"</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>205</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C37" s="6" t="str">
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Typical"</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>205</v>
+        <v>Amendment is determined to be "Complex"</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>196</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="8">
         <v>20</v>
@@ -10641,21 +10635,21 @@
         <v>Amendment is determined to be "Complex"</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>217</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="G38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="8">
         <v>20</v>
@@ -10664,70 +10658,70 @@
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is determined to be "Complex"</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>246</v>
+      <c r="D39" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C40" s="6" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Complex"</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>222</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="6" t="str">
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="8">
         <v>22</v>
@@ -10736,22 +10730,22 @@
         <f>IF((B42=""),"",VLOOKUP(B42,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D42" s="26" t="s">
-        <v>196</v>
+      <c r="D42" t="s">
+        <v>198</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="8">
         <v>22</v>
@@ -10760,46 +10754,46 @@
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D43" t="s">
-        <v>198</v>
+      <c r="D43" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C44" s="6" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="8">
         <v>23</v>
@@ -10808,22 +10802,22 @@
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D45" s="26" t="s">
-        <v>196</v>
+      <c r="D45" t="s">
+        <v>198</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G45" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="8">
         <v>23</v>
@@ -10832,70 +10826,70 @@
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D46" t="s">
-        <v>198</v>
+      <c r="D46" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G46" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" s="6" t="str">
         <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G47" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48" s="6" t="str">
         <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G48" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="8">
         <v>25</v>
@@ -10904,22 +10898,22 @@
         <f>IF((B49=""),"",VLOOKUP(B49,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D49" s="26" t="s">
-        <v>196</v>
+      <c r="D49" t="s">
+        <v>198</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G49" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" s="8">
         <v>25</v>
@@ -10928,46 +10922,46 @@
         <f>IF((B50=""),"",VLOOKUP(B50,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D50" t="s">
-        <v>198</v>
+      <c r="D50" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G50" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C51" s="6" t="str">
         <f>IF((B51=""),"",VLOOKUP(B51,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G51" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="8">
         <v>26</v>
@@ -10976,22 +10970,22 @@
         <f>IF((B52=""),"",VLOOKUP(B52,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D52" s="26" t="s">
-        <v>196</v>
+      <c r="D52" t="s">
+        <v>198</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G52" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="8">
         <v>26</v>
@@ -11000,70 +10994,70 @@
         <f>IF((B53=""),"",VLOOKUP(B53,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D53" t="s">
-        <v>198</v>
+      <c r="D53" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G53" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C54" s="6" t="str">
         <f>IF((B54=""),"",VLOOKUP(B54,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G54" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C55" s="6" t="str">
         <f>IF((B55=""),"",VLOOKUP(B55,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G55" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="8">
         <v>28</v>
@@ -11072,22 +11066,22 @@
         <f>IF((B56=""),"",VLOOKUP(B56,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D56" s="26" t="s">
-        <v>196</v>
+      <c r="D56" t="s">
+        <v>198</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G56" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="8">
         <v>28</v>
@@ -11096,46 +11090,46 @@
         <f>IF((B57=""),"",VLOOKUP(B57,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D57" t="s">
-        <v>198</v>
+      <c r="D57" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G57" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" s="6" t="str">
         <f>IF((B58=""),"",VLOOKUP(B58,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G58" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="8">
         <v>29</v>
@@ -11144,22 +11138,22 @@
         <f>IF((B59=""),"",VLOOKUP(B59,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D59" s="26" t="s">
-        <v>196</v>
+      <c r="D59" t="s">
+        <v>198</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G59" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="8">
         <v>29</v>
@@ -11168,46 +11162,46 @@
         <f>IF((B60=""),"",VLOOKUP(B60,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D60" t="s">
-        <v>198</v>
+      <c r="D60" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G60" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6" t="str">
         <f>IF((B61=""),"",VLOOKUP(B61,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="G61" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="8">
         <v>30</v>
@@ -11216,22 +11210,22 @@
         <f>IF((B62=""),"",VLOOKUP(B62,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D62" s="26" t="s">
-        <v>196</v>
+      <c r="D62" t="s">
+        <v>198</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G62" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="8">
         <v>30</v>
@@ -11240,88 +11234,64 @@
         <f>IF((B63=""),"",VLOOKUP(B63,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D63" t="s">
-        <v>198</v>
+      <c r="D63" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G63" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C64" s="6" t="str">
         <f>IF((B64=""),"",VLOOKUP(B64,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Decision Maker Amends the EAC/Exemption Order</v>
       </c>
       <c r="D64" s="26" t="s">
         <v>200</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G64" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" s="8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C65" s="6" t="str">
         <f>IF((B65=""),"",VLOOKUP(B65,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Decision Maker Amends the EAC/Exemption Order</v>
+        <v>Decision Maker Refuses to Amend the EAC/Exemption Order</v>
       </c>
       <c r="D65" s="26" t="s">
         <v>200</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G65" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>65</v>
-      </c>
-      <c r="B66" s="8">
-        <v>32</v>
-      </c>
-      <c r="C66" s="6" t="str">
-        <f>IF((B66=""),"",VLOOKUP(B66,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Decision Maker Refuses to Amend the EAC/Exemption Order</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G66" s="3">
         <v>65</v>
       </c>
     </row>
@@ -11334,7 +11304,7 @@
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$33</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B66</xm:sqref>
+          <xm:sqref>B2:B65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
addEvent action logic + event list sorting (#1364)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B63CD0-BE2E-4717-B9E1-C8A735F279F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD980EA4-B3C4-42B1-8728-5EDE39A9633A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="249">
   <si>
     <t>No</t>
   </si>
@@ -843,12 +843,6 @@
     <t>Set ANTICIPATED of "Amendment Application Submission | Amendment Application Received" to thisEventACTUAL +1</t>
   </si>
   <si>
-    <t>Add a copy of "Amendment Application Development (Proponent Time) | Submission of "Draft" Amendment Application" to thisPhase at thisEventACTUAL +28</t>
-  </si>
-  <si>
-    <t>Add a copy of "Amendment Application Development (Proponent Time) | "Draft" Amendment Application Initial Review" to thisPhase at thisEventACTUAL +38</t>
-  </si>
-  <si>
     <t>LockWorkStartDate</t>
   </si>
   <si>
@@ -906,12 +900,6 @@
     <t>{"work_state": "TERMINATED"}</t>
   </si>
   <si>
-    <t>{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Amendment Application", "start_at": 28 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "\"Draft\" Amendment Application Initial Review", "start_at": 38 }</t>
-  </si>
-  <si>
     <t>{"start_date_locked": true}</t>
   </si>
   <si>
@@ -967,6 +955,12 @@
   </si>
   <si>
     <t>[{"phase_name":"Amendment Application Review (Simple)","work_type_id": 7, "ea_act_id": 3, "new_name": "Amendment Application Review (Simple)", "legislated": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Amendment Application", "start_at": 28 },{"phase_name":"Amendment Application Development (Proponent Time)","work_type_id": 7, "ea_act_id": 3, "event_name": "\"Draft\" Amendment Application Initial Review", "start_at": 10}]</t>
+  </si>
+  <si>
+    <t>Add a copy of "Amendment Application Development (Proponent Time) | Submission of "Draft" Amendment Application, "Draft" Amendment Application Initial Review" to thisPhase at thisEventACTUAL +28</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1648,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1668,7 +1662,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
@@ -1683,7 +1677,7 @@
         <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1697,7 +1691,7 @@
         <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>20</v>
@@ -1712,7 +1706,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1726,7 +1720,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -1741,7 +1735,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I4" s="3">
         <v>3</v>
@@ -1755,7 +1749,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -1770,7 +1764,7 @@
         <v>65</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -1784,7 +1778,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -1799,7 +1793,7 @@
         <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
@@ -1813,7 +1807,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -1828,7 +1822,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
@@ -1842,7 +1836,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
@@ -1857,7 +1851,7 @@
         <v>65</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I8" s="3">
         <v>7</v>
@@ -1871,7 +1865,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -1886,7 +1880,7 @@
         <v>65</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I9" s="3">
         <v>8</v>
@@ -2584,7 +2578,7 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
@@ -2623,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M2" s="3">
         <v>1</v>
@@ -2662,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -2701,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
@@ -2740,7 +2734,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M5" s="3">
         <v>4</v>
@@ -2779,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M6" s="3">
         <v>5</v>
@@ -2818,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M7" s="3">
         <v>6</v>
@@ -2857,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M8" s="3">
         <v>7</v>
@@ -2896,7 +2890,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M9" s="3">
         <v>8</v>
@@ -2935,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M10" s="3">
         <v>9</v>
@@ -2974,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M11" s="3">
         <v>10</v>
@@ -3013,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M12" s="3">
         <v>11</v>
@@ -3052,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M13" s="3">
         <v>12</v>
@@ -3091,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M14" s="3">
         <v>13</v>
@@ -3130,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M15" s="3">
         <v>14</v>
@@ -3172,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M16" s="3">
         <v>15</v>
@@ -3214,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M17" s="3">
         <v>16</v>
@@ -3253,7 +3247,7 @@
         <v>30</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M18" s="3">
         <v>17</v>
@@ -3295,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M19" s="3">
         <v>18</v>
@@ -3337,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M20" s="3">
         <v>19</v>
@@ -3379,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M21" s="3">
         <v>20</v>
@@ -3421,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M22" s="3">
         <v>21</v>
@@ -3460,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M23" s="3">
         <v>22</v>
@@ -3499,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M24" s="3">
         <v>23</v>
@@ -3538,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M25" s="3">
         <v>24</v>
@@ -3580,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M26" s="3">
         <v>25</v>
@@ -3622,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M27" s="3">
         <v>26</v>
@@ -3661,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M28" s="3">
         <v>27</v>
@@ -3703,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M29" s="3">
         <v>28</v>
@@ -3745,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M30" s="3">
         <v>29</v>
@@ -3784,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M31" s="3">
         <v>30</v>
@@ -3826,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M32" s="3">
         <v>31</v>
@@ -3868,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M33" s="3">
         <v>32</v>
@@ -3907,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M34" s="3">
         <v>33</v>
@@ -3946,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M35" s="3">
         <v>34</v>
@@ -3988,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M36" s="3">
         <v>35</v>
@@ -4030,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M37" s="3">
         <v>36</v>
@@ -4069,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M38" s="3">
         <v>37</v>
@@ -4108,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M39" s="3">
         <v>38</v>
@@ -4147,7 +4141,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M40" s="3">
         <v>39</v>
@@ -4186,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M41" s="3">
         <v>40</v>
@@ -4225,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M42" s="3">
         <v>41</v>
@@ -4264,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M43" s="3">
         <v>42</v>
@@ -4303,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M44" s="3">
         <v>43</v>
@@ -4345,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M45" s="3">
         <v>44</v>
@@ -4387,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M46" s="3">
         <v>45</v>
@@ -4426,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M47" s="3">
         <v>46</v>
@@ -4468,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M48" s="3">
         <v>47</v>
@@ -4510,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M49" s="3">
         <v>48</v>
@@ -4549,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M50" s="3">
         <v>49</v>
@@ -4591,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M51" s="3">
         <v>50</v>
@@ -4633,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M52" s="3">
         <v>51</v>
@@ -4672,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M53" s="3">
         <v>52</v>
@@ -4711,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M54" s="3">
         <v>53</v>
@@ -4750,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M55" s="3">
         <v>54</v>
@@ -4792,7 +4786,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M56" s="3">
         <v>55</v>
@@ -4834,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M57" s="3">
         <v>56</v>
@@ -4873,7 +4867,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M58" s="3">
         <v>57</v>
@@ -4912,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M59" s="3">
         <v>58</v>
@@ -4954,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M60" s="3">
         <v>59</v>
@@ -4993,7 +4987,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M61" s="3">
         <v>60</v>
@@ -5032,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M62" s="3">
         <v>61</v>
@@ -5071,7 +5065,7 @@
         <v>0</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M63" s="3">
         <v>62</v>
@@ -5113,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M64" s="3">
         <v>63</v>
@@ -5155,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M65" s="3">
         <v>64</v>
@@ -5194,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M66" s="3">
         <v>65</v>
@@ -5236,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M67" s="3">
         <v>66</v>
@@ -5278,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M68" s="3">
         <v>67</v>
@@ -5317,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M69" s="3">
         <v>68</v>
@@ -5359,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M70" s="3">
         <v>69</v>
@@ -5401,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M71" s="3">
         <v>70</v>
@@ -5440,7 +5434,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M72" s="3">
         <v>71</v>
@@ -5479,7 +5473,7 @@
         <v>0</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M73" s="3">
         <v>72</v>
@@ -5518,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M74" s="3">
         <v>73</v>
@@ -5557,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M75" s="3">
         <v>74</v>
@@ -5596,7 +5590,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M76" s="3">
         <v>75</v>
@@ -5635,7 +5629,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M77" s="3">
         <v>76</v>
@@ -5674,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M78" s="3">
         <v>77</v>
@@ -5716,7 +5710,7 @@
         <v>0</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M79" s="3">
         <v>78</v>
@@ -5758,7 +5752,7 @@
         <v>0</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M80" s="3">
         <v>79</v>
@@ -5797,7 +5791,7 @@
         <v>30</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M81" s="3">
         <v>80</v>
@@ -5839,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M82" s="3">
         <v>81</v>
@@ -5881,7 +5875,7 @@
         <v>0</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M83" s="3">
         <v>82</v>
@@ -5923,7 +5917,7 @@
         <v>0</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M84" s="3">
         <v>83</v>
@@ -5965,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M85" s="3">
         <v>84</v>
@@ -6004,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M86" s="3">
         <v>85</v>
@@ -6043,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M87" s="3">
         <v>86</v>
@@ -6082,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M88" s="3">
         <v>87</v>
@@ -6124,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M89" s="3">
         <v>88</v>
@@ -6166,7 +6160,7 @@
         <v>0</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M90" s="3">
         <v>89</v>
@@ -6205,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M91" s="3">
         <v>90</v>
@@ -6247,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M92" s="3">
         <v>91</v>
@@ -6289,7 +6283,7 @@
         <v>0</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M93" s="3">
         <v>92</v>
@@ -6328,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M94" s="3">
         <v>93</v>
@@ -6370,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M95" s="3">
         <v>94</v>
@@ -6412,7 +6406,7 @@
         <v>0</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M96" s="3">
         <v>95</v>
@@ -6451,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M97" s="3">
         <v>96</v>
@@ -6490,7 +6484,7 @@
         <v>0</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M98" s="3">
         <v>97</v>
@@ -6529,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M99" s="3">
         <v>98</v>
@@ -6568,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M100" s="3">
         <v>99</v>
@@ -6607,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M101" s="3">
         <v>100</v>
@@ -6646,7 +6640,7 @@
         <v>0</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M102" s="3">
         <v>101</v>
@@ -6685,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M103" s="3">
         <v>102</v>
@@ -6724,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="L104" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M104" s="3">
         <v>103</v>
@@ -6766,7 +6760,7 @@
         <v>0</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M105" s="3">
         <v>104</v>
@@ -6808,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M106" s="3">
         <v>105</v>
@@ -6847,7 +6841,7 @@
         <v>30</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M107" s="3">
         <v>106</v>
@@ -6889,7 +6883,7 @@
         <v>0</v>
       </c>
       <c r="L108" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M108" s="3">
         <v>107</v>
@@ -6931,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="L109" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M109" s="3">
         <v>108</v>
@@ -6973,7 +6967,7 @@
         <v>0</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M110" s="3">
         <v>109</v>
@@ -7015,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="L111" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M111" s="3">
         <v>110</v>
@@ -7054,7 +7048,7 @@
         <v>0</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M112" s="3">
         <v>111</v>
@@ -7093,7 +7087,7 @@
         <v>0</v>
       </c>
       <c r="L113" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M113" s="3">
         <v>112</v>
@@ -7132,7 +7126,7 @@
         <v>0</v>
       </c>
       <c r="L114" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M114" s="3">
         <v>113</v>
@@ -7174,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M115" s="3">
         <v>114</v>
@@ -7216,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M116" s="3">
         <v>115</v>
@@ -7255,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M117" s="3">
         <v>116</v>
@@ -7297,7 +7291,7 @@
         <v>0</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M118" s="3">
         <v>117</v>
@@ -7339,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M119" s="3">
         <v>118</v>
@@ -7378,7 +7372,7 @@
         <v>0</v>
       </c>
       <c r="L120" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M120" s="3">
         <v>119</v>
@@ -7420,7 +7414,7 @@
         <v>0</v>
       </c>
       <c r="L121" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M121" s="3">
         <v>120</v>
@@ -7462,7 +7456,7 @@
         <v>0</v>
       </c>
       <c r="L122" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M122" s="3">
         <v>121</v>
@@ -7501,7 +7495,7 @@
         <v>0</v>
       </c>
       <c r="L123" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M123" s="3">
         <v>122</v>
@@ -7540,7 +7534,7 @@
         <v>0</v>
       </c>
       <c r="L124" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M124" s="3">
         <v>123</v>
@@ -7579,7 +7573,7 @@
         <v>0</v>
       </c>
       <c r="L125" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M125" s="3">
         <v>124</v>
@@ -7618,7 +7612,7 @@
         <v>0</v>
       </c>
       <c r="L126" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M126" s="3">
         <v>125</v>
@@ -7657,7 +7651,7 @@
         <v>0</v>
       </c>
       <c r="L127" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M127" s="3">
         <v>126</v>
@@ -7696,7 +7690,7 @@
         <v>0</v>
       </c>
       <c r="L128" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M128" s="3">
         <v>127</v>
@@ -7735,7 +7729,7 @@
         <v>0</v>
       </c>
       <c r="L129" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M129" s="3">
         <v>128</v>
@@ -7774,7 +7768,7 @@
         <v>0</v>
       </c>
       <c r="L130" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M130" s="3">
         <v>129</v>
@@ -7816,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="L131" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M131" s="3">
         <v>130</v>
@@ -7858,7 +7852,7 @@
         <v>0</v>
       </c>
       <c r="L132" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M132" s="3">
         <v>131</v>
@@ -7897,7 +7891,7 @@
         <v>30</v>
       </c>
       <c r="L133" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M133" s="3">
         <v>132</v>
@@ -7939,7 +7933,7 @@
         <v>0</v>
       </c>
       <c r="L134" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M134" s="3">
         <v>133</v>
@@ -7981,7 +7975,7 @@
         <v>0</v>
       </c>
       <c r="L135" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M135" s="3">
         <v>134</v>
@@ -8023,7 +8017,7 @@
         <v>0</v>
       </c>
       <c r="L136" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M136" s="3">
         <v>135</v>
@@ -8065,7 +8059,7 @@
         <v>0</v>
       </c>
       <c r="L137" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M137" s="3">
         <v>136</v>
@@ -8104,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="L138" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M138" s="3">
         <v>137</v>
@@ -8143,7 +8137,7 @@
         <v>0</v>
       </c>
       <c r="L139" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M139" s="3">
         <v>138</v>
@@ -8182,7 +8176,7 @@
         <v>0</v>
       </c>
       <c r="L140" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M140" s="3">
         <v>139</v>
@@ -8224,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="L141" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M141" s="3">
         <v>140</v>
@@ -8266,7 +8260,7 @@
         <v>0</v>
       </c>
       <c r="L142" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M142" s="3">
         <v>141</v>
@@ -8305,7 +8299,7 @@
         <v>0</v>
       </c>
       <c r="L143" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M143" s="3">
         <v>142</v>
@@ -8347,7 +8341,7 @@
         <v>0</v>
       </c>
       <c r="L144" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M144" s="3">
         <v>143</v>
@@ -8389,7 +8383,7 @@
         <v>0</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M145" s="3">
         <v>144</v>
@@ -8428,7 +8422,7 @@
         <v>0</v>
       </c>
       <c r="L146" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M146" s="3">
         <v>145</v>
@@ -8470,7 +8464,7 @@
         <v>0</v>
       </c>
       <c r="L147" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M147" s="3">
         <v>146</v>
@@ -8512,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="L148" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M148" s="3">
         <v>147</v>
@@ -8551,7 +8545,7 @@
         <v>0</v>
       </c>
       <c r="L149" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M149" s="3">
         <v>148</v>
@@ -8590,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M150" s="3">
         <v>149</v>
@@ -8629,7 +8623,7 @@
         <v>0</v>
       </c>
       <c r="L151" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M151" s="3">
         <v>150</v>
@@ -8668,7 +8662,7 @@
         <v>0</v>
       </c>
       <c r="L152" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M152" s="3">
         <v>151</v>
@@ -8710,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="L153" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M153" s="3">
         <v>152</v>
@@ -8749,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="L154" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M154" s="3">
         <v>153</v>
@@ -8788,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="L155" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M155" s="3">
         <v>154</v>
@@ -8830,7 +8824,7 @@
         <v>0</v>
       </c>
       <c r="L156" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M156" s="3">
         <v>155</v>
@@ -8872,7 +8866,7 @@
         <v>0</v>
       </c>
       <c r="L157" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M157" s="3">
         <v>156</v>
@@ -8911,7 +8905,7 @@
         <v>0</v>
       </c>
       <c r="L158" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M158" s="3">
         <v>157</v>
@@ -8950,7 +8944,7 @@
         <v>0</v>
       </c>
       <c r="L159" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M159" s="3">
         <v>158</v>
@@ -8992,7 +8986,7 @@
         <v>0</v>
       </c>
       <c r="L160" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M160" s="3">
         <v>159</v>
@@ -9034,7 +9028,7 @@
         <v>0</v>
       </c>
       <c r="L161" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M161" s="3">
         <v>160</v>
@@ -9721,13 +9715,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9783,7 +9777,7 @@
         <v>197</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -9807,7 +9801,7 @@
         <v>199</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -9831,7 +9825,7 @@
         <v>201</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -9855,7 +9849,7 @@
         <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -9879,7 +9873,7 @@
         <v>197</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -9903,7 +9897,7 @@
         <v>199</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -9927,7 +9921,7 @@
         <v>204</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
@@ -9951,7 +9945,7 @@
         <v>197</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -9975,7 +9969,7 @@
         <v>199</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -9999,7 +9993,7 @@
         <v>201</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -10023,7 +10017,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -10047,7 +10041,7 @@
         <v>208</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -10068,10 +10062,10 @@
         <v>207</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
@@ -10079,55 +10073,55 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="str">
         <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Initial Review of "Draft" Amendment Application is NEGATIVE</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>210</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6" t="str">
         <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="8">
         <v>9</v>
@@ -10136,22 +10130,22 @@
         <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>196</v>
+      <c r="D17" t="s">
+        <v>198</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G17" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8">
         <v>9</v>
@@ -10160,46 +10154,46 @@
         <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D18" t="s">
-        <v>198</v>
+      <c r="D18" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="6" t="str">
         <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="8">
         <v>10</v>
@@ -10208,22 +10202,22 @@
         <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D20" s="26" t="s">
-        <v>196</v>
+      <c r="D20" t="s">
+        <v>198</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="8">
         <v>10</v>
@@ -10232,166 +10226,166 @@
         <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D21" t="s">
-        <v>198</v>
+      <c r="D21" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="6" t="str">
         <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Starts the "clock" for Amendment</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>210</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>228</v>
       </c>
       <c r="G22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="6" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Starts the "clock" for Amendment</v>
+        <v>ADM, EA Operations is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>211</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="6" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>ADM, EA Operations is delegated to make the final Amendment Decision</v>
+        <v>CEAO is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D24" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>216</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="6" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>CEAO is delegated to make the final Amendment Decision</v>
+        <v>Minister is delegated to make the final Amendment Decision</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="6" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Minister is delegated to make the final Amendment Decision</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="G26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="6" t="str">
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="8">
         <v>16</v>
@@ -10400,22 +10394,22 @@
         <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>196</v>
+      <c r="D28" t="s">
+        <v>198</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="8">
         <v>16</v>
@@ -10424,46 +10418,46 @@
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D29" t="s">
-        <v>198</v>
+      <c r="D29" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="8">
         <v>17</v>
@@ -10472,22 +10466,22 @@
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D31" s="26" t="s">
-        <v>196</v>
+      <c r="D31" t="s">
+        <v>198</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="8">
         <v>17</v>
@@ -10496,46 +10490,46 @@
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D32" t="s">
-        <v>198</v>
+      <c r="D32" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="6" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="G33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="8">
         <v>18</v>
@@ -10545,21 +10539,21 @@
         <v>Amendment is determined to be "Simple"</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="8">
         <v>18</v>
@@ -10568,70 +10562,70 @@
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is determined to be "Simple"</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>246</v>
+      <c r="D35" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" s="6" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Simple"</v>
+        <v>Amendment is determined to be "Typical"</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>205</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C37" s="6" t="str">
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Typical"</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>205</v>
+        <v>Amendment is determined to be "Complex"</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>196</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="8">
         <v>20</v>
@@ -10641,21 +10635,21 @@
         <v>Amendment is determined to be "Complex"</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>217</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="G38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="8">
         <v>20</v>
@@ -10664,70 +10658,70 @@
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is determined to be "Complex"</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>246</v>
+      <c r="D39" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C40" s="6" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is determined to be "Complex"</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>222</v>
+        <v>Dispute Resolution is started</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="6" t="str">
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="8">
         <v>22</v>
@@ -10736,22 +10730,22 @@
         <f>IF((B42=""),"",VLOOKUP(B42,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D42" s="26" t="s">
-        <v>196</v>
+      <c r="D42" t="s">
+        <v>198</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="8">
         <v>22</v>
@@ -10760,46 +10754,46 @@
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D43" t="s">
-        <v>198</v>
+      <c r="D43" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C44" s="6" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="8">
         <v>23</v>
@@ -10808,22 +10802,22 @@
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D45" s="26" t="s">
-        <v>196</v>
+      <c r="D45" t="s">
+        <v>198</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G45" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="8">
         <v>23</v>
@@ -10832,70 +10826,70 @@
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D46" t="s">
-        <v>198</v>
+      <c r="D46" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G46" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" s="6" t="str">
         <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G47" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48" s="6" t="str">
         <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G48" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="8">
         <v>25</v>
@@ -10904,22 +10898,22 @@
         <f>IF((B49=""),"",VLOOKUP(B49,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D49" s="26" t="s">
-        <v>196</v>
+      <c r="D49" t="s">
+        <v>198</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G49" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" s="8">
         <v>25</v>
@@ -10928,46 +10922,46 @@
         <f>IF((B50=""),"",VLOOKUP(B50,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D50" t="s">
-        <v>198</v>
+      <c r="D50" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G50" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C51" s="6" t="str">
         <f>IF((B51=""),"",VLOOKUP(B51,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G51" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="8">
         <v>26</v>
@@ -10976,22 +10970,22 @@
         <f>IF((B52=""),"",VLOOKUP(B52,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D52" s="26" t="s">
-        <v>196</v>
+      <c r="D52" t="s">
+        <v>198</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G52" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="8">
         <v>26</v>
@@ -11000,70 +10994,70 @@
         <f>IF((B53=""),"",VLOOKUP(B53,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D53" t="s">
-        <v>198</v>
+      <c r="D53" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G53" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C54" s="6" t="str">
         <f>IF((B54=""),"",VLOOKUP(B54,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Dispute Resolution is started</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G54" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C55" s="6" t="str">
         <f>IF((B55=""),"",VLOOKUP(B55,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Dispute Resolution is started</v>
+        <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G55" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="8">
         <v>28</v>
@@ -11072,22 +11066,22 @@
         <f>IF((B56=""),"",VLOOKUP(B56,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D56" s="26" t="s">
-        <v>196</v>
+      <c r="D56" t="s">
+        <v>198</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G56" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="8">
         <v>28</v>
@@ -11096,46 +11090,46 @@
         <f>IF((B57=""),"",VLOOKUP(B57,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Amendment is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D57" t="s">
-        <v>198</v>
+      <c r="D57" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G57" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" s="6" t="str">
         <f>IF((B58=""),"",VLOOKUP(B58,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Amendment is Terminated under s.39(d) of Act</v>
+        <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>204</v>
+        <v>196</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G58" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="8">
         <v>29</v>
@@ -11144,22 +11138,22 @@
         <f>IF((B59=""),"",VLOOKUP(B59,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D59" s="26" t="s">
-        <v>196</v>
+      <c r="D59" t="s">
+        <v>198</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G59" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="8">
         <v>29</v>
@@ -11168,46 +11162,46 @@
         <f>IF((B60=""),"",VLOOKUP(B60,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D60" t="s">
-        <v>198</v>
+      <c r="D60" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G60" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6" t="str">
         <f>IF((B61=""),"",VLOOKUP(B61,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="G61" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="8">
         <v>30</v>
@@ -11216,22 +11210,22 @@
         <f>IF((B62=""),"",VLOOKUP(B62,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D62" s="26" t="s">
-        <v>196</v>
+      <c r="D62" t="s">
+        <v>198</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G62" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="8">
         <v>30</v>
@@ -11240,88 +11234,64 @@
         <f>IF((B63=""),"",VLOOKUP(B63,Outcomes!$A$2:$D$33,4,FALSE))</f>
         <v>Holder withdraws Application from Amendment process</v>
       </c>
-      <c r="D63" t="s">
-        <v>198</v>
+      <c r="D63" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G63" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C64" s="6" t="str">
         <f>IF((B64=""),"",VLOOKUP(B64,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Holder withdraws Application from Amendment process</v>
+        <v>Decision Maker Amends the EAC/Exemption Order</v>
       </c>
       <c r="D64" s="26" t="s">
         <v>200</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G64" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" s="8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C65" s="6" t="str">
         <f>IF((B65=""),"",VLOOKUP(B65,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Decision Maker Amends the EAC/Exemption Order</v>
+        <v>Decision Maker Refuses to Amend the EAC/Exemption Order</v>
       </c>
       <c r="D65" s="26" t="s">
         <v>200</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G65" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>65</v>
-      </c>
-      <c r="B66" s="8">
-        <v>32</v>
-      </c>
-      <c r="C66" s="6" t="str">
-        <f>IF((B66=""),"",VLOOKUP(B66,Outcomes!$A$2:$D$33,4,FALSE))</f>
-        <v>Decision Maker Refuses to Amend the EAC/Exemption Order</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G66" s="3">
         <v>65</v>
       </c>
     </row>
@@ -11334,7 +11304,7 @@
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$33</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B66</xm:sqref>
+          <xm:sqref>B2:B65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
UserList changes, Group fetching logic changes based on changes in keycloak (#1462)
* User list changes for the kc changes

* review comments

* review feedbacks
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/001_Amendment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD980EA4-B3C4-42B1-8728-5EDE39A9633A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B9FD62-E0A7-4FB1-9CD5-44D68F667280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Actions" sheetId="6" r:id="rId5"/>
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$65</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1545,55 +1548,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.5">
       <c r="B12" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>64</v>
       </c>
@@ -1614,18 +1617,18 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.77734375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="12.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.81640625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="12.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1886,607 +1889,607 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B99"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B114"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B116"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B119"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B120"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B121"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B123"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B124"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B125"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B126"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B127"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B128"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B129"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B130"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B131"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B132"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B133"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B134"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B135"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B136"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B137"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B138"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B139"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B140"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B141"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B142"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B143"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B144"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B145"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B146"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B147"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B148"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B149"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B150"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B151"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B152"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B153"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B154"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B155"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B156"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B157"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B158"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B159"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B160"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B161"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B162"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B163"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B164"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B165"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B166"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B167"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B168"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B169"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B170"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B171"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B172"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B173"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B174"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B175"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B176"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B177"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B178"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B179"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B180"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B181"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B182"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B183"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B184"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B185"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B186"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B187"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B188"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B189"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B190"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B191"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B192"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B193"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B194"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B195"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B196"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B197"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B198"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B199"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B200"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B201"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B202"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B203"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B204"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B205"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B206"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B207"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B208"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B209"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B210"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B211"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B212"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B213"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B214"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B215"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B216"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B217"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B218"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B219"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B220"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B221"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B222"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B223"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B224"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B225"/>
     </row>
   </sheetData>
@@ -2529,21 +2532,21 @@
       <selection pane="bottomRight" activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="62.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="14.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.81640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.81640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="62.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" style="2" customWidth="1"/>
+    <col min="11" max="12" width="14.81640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.81640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2662,7 +2665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2740,7 +2743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3091,7 +3094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3295,7 +3298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3379,7 +3382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3421,7 +3424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3538,7 +3541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3703,7 +3706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3784,7 +3787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3826,7 +3829,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3868,7 +3871,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3907,7 +3910,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3988,7 +3991,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4147,7 +4150,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4225,7 +4228,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4264,7 +4267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4303,7 +4306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4345,7 +4348,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4387,7 +4390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4426,7 +4429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4468,7 +4471,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4510,7 +4513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4549,7 +4552,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4591,7 +4594,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4633,7 +4636,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4672,7 +4675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4711,7 +4714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4750,7 +4753,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4792,7 +4795,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4834,7 +4837,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4873,7 +4876,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4912,7 +4915,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4954,7 +4957,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5032,7 +5035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5113,7 +5116,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5155,7 +5158,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5194,7 +5197,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5236,7 +5239,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5278,7 +5281,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5359,7 +5362,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5401,7 +5404,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5479,7 +5482,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5518,7 +5521,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5635,7 +5638,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5674,7 +5677,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5797,7 +5800,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -5839,7 +5842,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -5923,7 +5926,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -5965,7 +5968,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -6004,7 +6007,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -6043,7 +6046,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -6082,7 +6085,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -6124,7 +6127,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -6247,7 +6250,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -6289,7 +6292,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -6328,7 +6331,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -6370,7 +6373,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -6412,7 +6415,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -6451,7 +6454,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -6490,7 +6493,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -6529,7 +6532,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -6568,7 +6571,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -6607,7 +6610,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -6646,7 +6649,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -6685,7 +6688,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -6724,7 +6727,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -6766,7 +6769,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -6808,7 +6811,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -6847,7 +6850,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -6889,7 +6892,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -6931,7 +6934,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -7015,7 +7018,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -7054,7 +7057,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -7093,7 +7096,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -7132,7 +7135,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -7174,7 +7177,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -7216,7 +7219,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -7255,7 +7258,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -7297,7 +7300,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -7339,7 +7342,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -7420,7 +7423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -7501,7 +7504,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -7540,7 +7543,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -7579,7 +7582,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -7618,7 +7621,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -7657,7 +7660,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -7696,7 +7699,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -7735,7 +7738,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -7774,7 +7777,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -7816,7 +7819,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -7858,7 +7861,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -7939,7 +7942,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -7981,7 +7984,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -8023,7 +8026,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -8065,7 +8068,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -8104,7 +8107,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -8143,7 +8146,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -8182,7 +8185,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -8224,7 +8227,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -8266,7 +8269,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -8305,7 +8308,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -8347,7 +8350,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -8428,7 +8431,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -8470,7 +8473,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -8512,7 +8515,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -8551,7 +8554,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -8590,7 +8593,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -8629,7 +8632,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -8668,7 +8671,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -8710,7 +8713,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -8749,7 +8752,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -8788,7 +8791,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -8830,7 +8833,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -8872,7 +8875,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -8911,7 +8914,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -8950,7 +8953,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -8992,7 +8995,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -9094,16 +9097,16 @@
       <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9120,7 +9123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -9138,7 +9141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -9156,7 +9159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -9174,7 +9177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -9192,7 +9195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -9210,7 +9213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -9228,7 +9231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -9246,7 +9249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -9264,7 +9267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -9282,7 +9285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -9300,7 +9303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -9318,7 +9321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -9336,7 +9339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -9354,7 +9357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -9372,7 +9375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9390,7 +9393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -9408,7 +9411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -9426,7 +9429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -9444,7 +9447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -9462,7 +9465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -9480,7 +9483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -9498,7 +9501,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -9516,7 +9519,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -9534,7 +9537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9552,7 +9555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9570,7 +9573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9588,7 +9591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9606,7 +9609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9624,7 +9627,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9642,7 +9645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9660,7 +9663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9678,7 +9681,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9718,25 +9721,25 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="2"/>
+    <col min="2" max="2" width="12.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="170" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="20.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9759,7 +9762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -9783,7 +9786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -9807,7 +9810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -9831,7 +9834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -9855,7 +9858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -9879,7 +9882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -9903,7 +9906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -9927,7 +9930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -9951,7 +9954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -9975,7 +9978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -9999,7 +10002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -10023,7 +10026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -10047,7 +10050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -10071,7 +10074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -10095,7 +10098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -10119,7 +10122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -10143,7 +10146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -10167,7 +10170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -10191,7 +10194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -10215,7 +10218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -10239,7 +10242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -10263,7 +10266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -10287,7 +10290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -10311,7 +10314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -10335,7 +10338,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -10359,7 +10362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -10383,7 +10386,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -10407,7 +10410,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -10431,7 +10434,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -10479,7 +10482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -10503,7 +10506,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -10527,7 +10530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -10551,7 +10554,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -10575,7 +10578,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -10599,7 +10602,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -10623,7 +10626,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -10647,7 +10650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -10671,7 +10674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -10695,7 +10698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -10719,7 +10722,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -10743,7 +10746,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>43</v>
       </c>
@@ -10767,7 +10770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>44</v>
       </c>
@@ -10791,7 +10794,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -10815,7 +10818,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -10839,7 +10842,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>47</v>
       </c>
@@ -10863,7 +10866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -10887,7 +10890,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>49</v>
       </c>
@@ -10911,7 +10914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>50</v>
       </c>
@@ -10935,7 +10938,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -10959,7 +10962,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -10983,7 +10986,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -11007,7 +11010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -11031,7 +11034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -11055,7 +11058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -11079,7 +11082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -11103,7 +11106,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>58</v>
       </c>
@@ -11127,7 +11130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -11151,7 +11154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -11175,7 +11178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>61</v>
       </c>
@@ -11199,7 +11202,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -11223,7 +11226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -11247,7 +11250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>64</v>
       </c>
@@ -11271,7 +11274,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -11296,6 +11299,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G65" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -11321,34 +11325,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.77734375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.77734375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.77734375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.77734375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.77734375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.77734375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.81640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.81640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.81640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.81640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.81640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.81640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.81640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.81640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.81640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.90625" style="4"/>
+    <col min="60" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -11427,7 +11431,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -11459,7 +11463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -11491,7 +11495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
@@ -11514,7 +11518,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -11531,7 +11535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>104</v>
       </c>
@@ -11548,7 +11552,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -11565,7 +11569,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
@@ -11582,7 +11586,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -11596,7 +11600,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -11608,7 +11612,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -11620,7 +11624,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -11632,7 +11636,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -11644,7 +11648,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -11656,7 +11660,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -11667,7 +11671,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
@@ -11675,7 +11679,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H18" s="4" t="s">
         <v>36</v>
       </c>
@@ -11683,7 +11687,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H19" s="4" t="s">
         <v>36</v>
       </c>
@@ -11691,7 +11695,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H20" s="4" t="s">
         <v>36</v>
       </c>
@@ -11699,7 +11703,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H21" s="4" t="s">
         <v>36</v>
       </c>
@@ -11707,7 +11711,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H22" s="4" t="s">
         <v>36</v>
       </c>
@@ -11715,7 +11719,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H23" s="4" t="s">
         <v>36</v>
       </c>
@@ -11723,7 +11727,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H24" s="4" t="s">
         <v>36</v>
       </c>
@@ -11731,7 +11735,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H25" s="4" t="s">
         <v>36</v>
       </c>
@@ -11739,7 +11743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H26" s="4" t="s">
         <v>38</v>
       </c>
@@ -11747,7 +11751,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H27" s="4" t="s">
         <v>38</v>
       </c>
@@ -11755,7 +11759,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H28" s="4" t="s">
         <v>38</v>
       </c>
@@ -11763,7 +11767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H29" s="4" t="s">
         <v>38</v>
       </c>
@@ -11771,7 +11775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H30" s="4" t="s">
         <v>35</v>
       </c>
@@ -11779,7 +11783,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H31" s="4" t="s">
         <v>35</v>
       </c>
@@ -11787,7 +11791,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H32" s="4" t="s">
         <v>35</v>
       </c>
@@ -11795,7 +11799,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H33" s="4" t="s">
         <v>35</v>
       </c>
@@ -11803,7 +11807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H34" s="4" t="s">
         <v>35</v>
       </c>
@@ -11811,7 +11815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H35" s="4" t="s">
         <v>37</v>
       </c>
@@ -11819,7 +11823,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H36" s="4" t="s">
         <v>37</v>
       </c>
@@ -11827,7 +11831,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H37" s="4" t="s">
         <v>37</v>
       </c>
@@ -11835,7 +11839,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H38" s="4" t="s">
         <v>37</v>
       </c>
@@ -11843,7 +11847,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H39" s="4" t="s">
         <v>37</v>
       </c>

</xml_diff>